<commit_message>
Cambios anotados en tutoria
</commit_message>
<xml_diff>
--- a/Documentacion/Planificacion - Gantt.xlsx
+++ b/Documentacion/Planificacion - Gantt.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nico/Lic.Informatica/Taller12019/Documentacion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpouso\Documents\Mathias\Taller 1 2019\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF7A6D5-8FCB-431C-9ECA-5D0FD9696B76}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39040" yWindow="440" windowWidth="36560" windowHeight="19640" tabRatio="500"/>
+    <workbookView xWindow="39045" yWindow="435" windowWidth="36555" windowHeight="19635" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -101,24 +102,6 @@
     <t>Implementación Módulo ABBPolinomio</t>
   </si>
   <si>
-    <t>Testing Módulo String</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Testing Módulo ListaParametros</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Testing Módulo Termino</t>
-  </si>
-  <si>
-    <t>Testing Módulo ListaTerminos</t>
-  </si>
-  <si>
-    <t>Testing Módulo Polinomio</t>
-  </si>
-  <si>
-    <t>Testing Módulo ABBPolinomio</t>
-  </si>
-  <si>
     <t xml:space="preserve">              - Comando Crear</t>
   </si>
   <si>
@@ -150,12 +133,30 @@
   </si>
   <si>
     <t>FEBRERO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Testing y Re-trabajo Módulo String</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Testing y Re-trabajo Módulo ListaParametros</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Testing y Re-trabajo Módulo Termino</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Testing y Re-trabajo Módulo ListaTerminos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Testing y Re-trabajo Módulo Polinomio</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Testing y Re-trabajo Módulo ABBPolinomio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -959,6 +960,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1226,31 +1230,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AS50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" showRuler="0" view="pageLayout" zoomScale="90" zoomScaleNormal="110" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.5" customWidth="1"/>
-    <col min="2" max="40" width="3.1640625" style="2" customWidth="1"/>
+    <col min="2" max="40" width="3.125" style="2" customWidth="1"/>
     <col min="41" max="41" width="7.5" style="2" customWidth="1"/>
-    <col min="42" max="42" width="7.6640625" style="2" customWidth="1"/>
-    <col min="43" max="43" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="3.1640625" style="2" customWidth="1"/>
-    <col min="45" max="101" width="3.1640625" customWidth="1"/>
+    <col min="42" max="42" width="7.625" style="2" customWidth="1"/>
+    <col min="43" max="43" width="7.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="3.125" style="2" customWidth="1"/>
+    <col min="45" max="101" width="3.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:45" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8"/>
       <c r="B1" s="74" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C1" s="75"/>
       <c r="D1" s="75"/>
@@ -1298,7 +1302,7 @@
       <c r="AP1" s="78"/>
       <c r="AQ1" s="79"/>
     </row>
-    <row r="2" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
       <c r="B2" s="30" t="s">
         <v>13</v>
@@ -1429,7 +1433,7 @@
       <c r="AR2" s="3"/>
       <c r="AS2" s="1"/>
     </row>
-    <row r="3" spans="1:45" s="2" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:45" s="2" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
@@ -1554,7 +1558,7 @@
       <c r="AP3" s="38"/>
       <c r="AQ3" s="39"/>
     </row>
-    <row r="4" spans="1:45" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:45" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>4</v>
       </c>
@@ -1601,7 +1605,7 @@
       <c r="AP4" s="41"/>
       <c r="AQ4" s="42"/>
     </row>
-    <row r="5" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>3</v>
       </c>
@@ -1648,7 +1652,7 @@
       <c r="AP5" s="4"/>
       <c r="AQ5" s="6"/>
     </row>
-    <row r="6" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>2</v>
       </c>
@@ -1695,9 +1699,9 @@
       <c r="AP6" s="36"/>
       <c r="AQ6" s="44"/>
     </row>
-    <row r="7" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B7" s="24"/>
       <c r="C7" s="58"/>
@@ -1742,9 +1746,9 @@
       <c r="AP7" s="5"/>
       <c r="AQ7" s="44"/>
     </row>
-    <row r="8" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B8" s="24"/>
       <c r="C8" s="58"/>
@@ -1789,9 +1793,9 @@
       <c r="AP8" s="36"/>
       <c r="AQ8" s="7"/>
     </row>
-    <row r="9" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B9" s="24"/>
       <c r="C9" s="58"/>
@@ -1836,9 +1840,9 @@
       <c r="AP9" s="4"/>
       <c r="AQ9" s="44"/>
     </row>
-    <row r="10" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B10" s="24"/>
       <c r="C10" s="58"/>
@@ -1883,9 +1887,9 @@
       <c r="AP10" s="36"/>
       <c r="AQ10" s="6"/>
     </row>
-    <row r="11" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B11" s="24"/>
       <c r="C11" s="58"/>
@@ -1930,9 +1934,9 @@
       <c r="AP11" s="4"/>
       <c r="AQ11" s="6"/>
     </row>
-    <row r="12" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B12" s="24"/>
       <c r="C12" s="58"/>
@@ -1977,9 +1981,9 @@
       <c r="AP12" s="4"/>
       <c r="AQ12" s="44"/>
     </row>
-    <row r="13" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B13" s="24"/>
       <c r="C13" s="58"/>
@@ -2024,9 +2028,9 @@
       <c r="AP13" s="36"/>
       <c r="AQ13" s="44"/>
     </row>
-    <row r="14" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B14" s="24"/>
       <c r="C14" s="58"/>
@@ -2071,7 +2075,7 @@
       <c r="AP14" s="36"/>
       <c r="AQ14" s="6"/>
     </row>
-    <row r="15" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>5</v>
       </c>
@@ -2118,7 +2122,7 @@
       <c r="AP15" s="4"/>
       <c r="AQ15" s="44"/>
     </row>
-    <row r="16" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
         <v>6</v>
       </c>
@@ -2165,7 +2169,7 @@
       <c r="AP16" s="4"/>
       <c r="AQ16" s="44"/>
     </row>
-    <row r="17" spans="1:43" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:43" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>7</v>
       </c>
@@ -2212,7 +2216,7 @@
       <c r="AP17" s="36"/>
       <c r="AQ17" s="44"/>
     </row>
-    <row r="18" spans="1:43" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:43" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>19</v>
       </c>
@@ -2259,9 +2263,9 @@
       <c r="AP18" s="36"/>
       <c r="AQ18" s="6"/>
     </row>
-    <row r="19" spans="1:43" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:43" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B19" s="24"/>
       <c r="C19" s="58"/>
@@ -2306,7 +2310,7 @@
       <c r="AP19" s="36"/>
       <c r="AQ19" s="6"/>
     </row>
-    <row r="20" spans="1:43" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:43" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>20</v>
       </c>
@@ -2353,9 +2357,9 @@
       <c r="AP20" s="36"/>
       <c r="AQ20" s="44"/>
     </row>
-    <row r="21" spans="1:43" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:43" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B21" s="24"/>
       <c r="C21" s="58"/>
@@ -2400,7 +2404,7 @@
       <c r="AP21" s="4"/>
       <c r="AQ21" s="6"/>
     </row>
-    <row r="22" spans="1:43" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:43" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
         <v>21</v>
       </c>
@@ -2447,9 +2451,9 @@
       <c r="AP22" s="4"/>
       <c r="AQ22" s="6"/>
     </row>
-    <row r="23" spans="1:43" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:43" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="B23" s="24"/>
       <c r="C23" s="58"/>
@@ -2494,7 +2498,7 @@
       <c r="AP23" s="4"/>
       <c r="AQ23" s="6"/>
     </row>
-    <row r="24" spans="1:43" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:43" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>22</v>
       </c>
@@ -2541,9 +2545,9 @@
       <c r="AP24" s="4"/>
       <c r="AQ24" s="44"/>
     </row>
-    <row r="25" spans="1:43" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:43" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B25" s="24"/>
       <c r="C25" s="58"/>
@@ -2588,7 +2592,7 @@
       <c r="AP25" s="4"/>
       <c r="AQ25" s="44"/>
     </row>
-    <row r="26" spans="1:43" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:43" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>23</v>
       </c>
@@ -2635,9 +2639,9 @@
       <c r="AP26" s="36"/>
       <c r="AQ26" s="44"/>
     </row>
-    <row r="27" spans="1:43" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:43" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B27" s="24"/>
       <c r="C27" s="58"/>
@@ -2682,9 +2686,9 @@
       <c r="AP27" s="36"/>
       <c r="AQ27" s="44"/>
     </row>
-    <row r="28" spans="1:43" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:43" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="B28" s="24"/>
       <c r="C28" s="58"/>
@@ -2729,7 +2733,7 @@
       <c r="AP28" s="36"/>
       <c r="AQ28" s="44"/>
     </row>
-    <row r="29" spans="1:43" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:43" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>24</v>
       </c>
@@ -2776,9 +2780,9 @@
       <c r="AP29" s="36"/>
       <c r="AQ29" s="44"/>
     </row>
-    <row r="30" spans="1:43" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:43" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B30" s="24"/>
       <c r="C30" s="58"/>
@@ -2823,9 +2827,9 @@
       <c r="AP30" s="36"/>
       <c r="AQ30" s="44"/>
     </row>
-    <row r="31" spans="1:43" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:43" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B31" s="24"/>
       <c r="C31" s="58"/>
@@ -2870,9 +2874,9 @@
       <c r="AP31" s="36"/>
       <c r="AQ31" s="44"/>
     </row>
-    <row r="32" spans="1:43" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:43" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="15" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B32" s="26"/>
       <c r="C32" s="59"/>
@@ -2917,24 +2921,24 @@
       <c r="AP32" s="48"/>
       <c r="AQ32" s="49"/>
     </row>
-    <row r="33" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:AB1"/>
@@ -2943,6 +2947,6 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="65" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" scale="54" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>